<commit_message>
update test-unit version_1.1 - NOT YET!
</commit_message>
<xml_diff>
--- a/TestFunctions.xlsx
+++ b/TestFunctions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOANG DUY\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CD34ED-13F0-424A-A134-DEAD86982124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568F64AA-FA60-4B32-95B3-F42A815BBD9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="277">
   <si>
     <t>Chức năng</t>
   </si>
@@ -599,6 +599,340 @@
   </si>
   <si>
     <t>Hiển thị danh sách các chức năng admin</t>
+  </si>
+  <si>
+    <t>Quản lí user</t>
+  </si>
+  <si>
+    <t>Click vào "Trang cms"</t>
+  </si>
+  <si>
+    <t>Hiển thị trang cms</t>
+  </si>
+  <si>
+    <t>Click vào tab "Quản lý user"</t>
+  </si>
+  <si>
+    <t>Hiển thị trang quản lí user</t>
+  </si>
+  <si>
+    <t>Click vào "Thêm người dùng mới"</t>
+  </si>
+  <si>
+    <t>Hiển thị phần khung thêm người dùng mới</t>
+  </si>
+  <si>
+    <t>Điền vô khung với username, password 
+và phone hợp lệ</t>
+  </si>
+  <si>
+    <t>Thêm người dùng mới
+thành công</t>
+  </si>
+  <si>
+    <t>Click nút "Submit"</t>
+  </si>
+  <si>
+    <t>Chọn vai trò user trong phần role</t>
+  </si>
+  <si>
+    <t>1 user mới được thêm vào
+ database và hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Điền vô khung với username, password 
+và phone không hợp lệ</t>
+  </si>
+  <si>
+    <t>Thêm người dùng mới
+thất bại</t>
+  </si>
+  <si>
+    <t>Func 20</t>
+  </si>
+  <si>
+    <t>Xoá user</t>
+  </si>
+  <si>
+    <t>1 user bị xoá khỏi
+ database và hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Func 21</t>
+  </si>
+  <si>
+    <t>Sửa user thành công</t>
+  </si>
+  <si>
+    <t>Click vào "Xoá" ứng với user muốn xoá</t>
+  </si>
+  <si>
+    <t>Click vào "Sửa" ứng với user muốn sửa</t>
+  </si>
+  <si>
+    <t>Hiển thị phần khung sửa user</t>
+  </si>
+  <si>
+    <t>Điền vô khung với new password 
+và phone không hợp lệ</t>
+  </si>
+  <si>
+    <t>Click nút "Sửa"</t>
+  </si>
+  <si>
+    <t>Func 22</t>
+  </si>
+  <si>
+    <t>Sửa user thất bại</t>
+  </si>
+  <si>
+    <t>Thông tin mới user được
+cập nhật vào database và
+hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Điền vô khung với new password 
+và phone hợp lệ</t>
+  </si>
+  <si>
+    <t>Sửa user thất bại và
+hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Quản lí vendor</t>
+  </si>
+  <si>
+    <t>Func 23</t>
+  </si>
+  <si>
+    <t>Thêm vendor mới
+thành công</t>
+  </si>
+  <si>
+    <t>Thêm vendor mới
+thất bại</t>
+  </si>
+  <si>
+    <t>Click vào tab "Quản lý vendor/thu ngân"</t>
+  </si>
+  <si>
+    <t>Hiển thị trang quản lí vendor/thu ngân</t>
+  </si>
+  <si>
+    <t>Click vào "Thêm vendor mới"</t>
+  </si>
+  <si>
+    <t>Hiển thị phần khung thêm vendor mới</t>
+  </si>
+  <si>
+    <t>Điền vô khung với 
+UsernameOwner, Password, 
+Số điện thoại và Tên quầy hợp lệ</t>
+  </si>
+  <si>
+    <t>Điền vô khung với 
+UsernameOwner, Password, 
+Số điện thoại và Tên quầy không hợp lệ</t>
+  </si>
+  <si>
+    <t>Click nút "Thêm"</t>
+  </si>
+  <si>
+    <t>Click vào tab "Vendor"</t>
+  </si>
+  <si>
+    <t>Hiển thị trang quản lí vendor</t>
+  </si>
+  <si>
+    <t>1 vendor mới được thêm vào
+ database và hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Thêm người dùng mới
+thất bại và hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Thêm vendor mới
+thất bại và hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>chưa check trùng pw cũ</t>
+  </si>
+  <si>
+    <t>Func 24</t>
+  </si>
+  <si>
+    <t>Func 25</t>
+  </si>
+  <si>
+    <t>Click vào "Sửa" ứng với vendor muốn sửa</t>
+  </si>
+  <si>
+    <t>Hiển thị phần khung sửa vendor</t>
+  </si>
+  <si>
+    <t>Sửa vendor thành công</t>
+  </si>
+  <si>
+    <t>Điền vô khung với UsernameOwner hợp lệ</t>
+  </si>
+  <si>
+    <t>Chọn trạng thái vendor</t>
+  </si>
+  <si>
+    <t>Click nút "Cập nhật"</t>
+  </si>
+  <si>
+    <t>Thông tin mới vendor được
+cập nhật vào database và
+hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>chưa check tên rỗng</t>
+  </si>
+  <si>
+    <t>Sửa vendor thất bại và
+hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Sửa vendor thất bại</t>
+  </si>
+  <si>
+    <t>Func 26</t>
+  </si>
+  <si>
+    <t>Điền vô khung với UsernameOwner
+không hợp lệ</t>
+  </si>
+  <si>
+    <t>Quản lí thu ngân</t>
+  </si>
+  <si>
+    <t>Func 27</t>
+  </si>
+  <si>
+    <t>Click vào tab "Thu ngân"</t>
+  </si>
+  <si>
+    <t>Hiển thị trang quản lí thu ngân</t>
+  </si>
+  <si>
+    <t>Click vào "Thêm thu ngân"</t>
+  </si>
+  <si>
+    <t>Hiển thị phần khung thêm thu ngân mới</t>
+  </si>
+  <si>
+    <t>Điền vô khung với UsernameOwner, Password và Số điện thoại hợp lệ</t>
+  </si>
+  <si>
+    <t>Thêm thu ngân mới
+thành công</t>
+  </si>
+  <si>
+    <t>1 thu ngân mới được thêm vào
+ database và hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Điền vô khung với UsernameOwner, Password và Số điện thoại không hợp lệ</t>
+  </si>
+  <si>
+    <t>Func 28</t>
+  </si>
+  <si>
+    <t>Thêm thu ngân mới
+thất bại</t>
+  </si>
+  <si>
+    <t>Thêm thu ngân mới
+thất bại và hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Func 29</t>
+  </si>
+  <si>
+    <t>Sửa trạng thái thu ngân</t>
+  </si>
+  <si>
+    <t>Click vào "Sửa" ứng với thu ngân muốn sửa</t>
+  </si>
+  <si>
+    <t>Hiển thị phần khung sửa thu ngân</t>
+  </si>
+  <si>
+    <t>Chọn trạng thái thu ngân</t>
+  </si>
+  <si>
+    <t>Thông tin mới thu ngân được
+cập nhật vào database và
+hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Bảo trì</t>
+  </si>
+  <si>
+    <t>Func 30</t>
+  </si>
+  <si>
+    <t>Bật bảo trì</t>
+  </si>
+  <si>
+    <t>Click vào tab "Bảo trì"</t>
+  </si>
+  <si>
+    <t>Hiển thị trang quản lí bảo trì</t>
+  </si>
+  <si>
+    <t>Click vào "Bật bảo trì"</t>
+  </si>
+  <si>
+    <t>Hệ thống vào trạng thái bảo trì
+và hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Tắt bảo trì</t>
+  </si>
+  <si>
+    <t>Func 31</t>
+  </si>
+  <si>
+    <t>Click vào "Tắt bảo trì"</t>
+  </si>
+  <si>
+    <t>Hệ thống thoát khỏi 
+trạng thái bảo trì và 
+hiển thị thông báo</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Func 32</t>
+  </si>
+  <si>
+    <t>Xem feedback</t>
+  </si>
+  <si>
+    <t>Click vào tab "Feedback"</t>
+  </si>
+  <si>
+    <t>Hiển thị trang feedback</t>
+  </si>
+  <si>
+    <t>Xem feedback thành công</t>
+  </si>
+  <si>
+    <t>Search feedback</t>
+  </si>
+  <si>
+    <t>Điền thông tin cần tìm vào ô Search
+bên góc phải</t>
+  </si>
+  <si>
+    <t>Func 33</t>
+  </si>
+  <si>
+    <t>Search feedback thành công</t>
   </si>
 </sst>
 </file>
@@ -762,7 +1096,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -794,120 +1128,135 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1249,9 +1598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1304,107 +1655,107 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="21"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" s="26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+    </row>
+    <row r="8" spans="1:8" s="15" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="28"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="29"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="31"/>
+      <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="25" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1413,61 +1764,61 @@
       <c r="E12" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="47"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="47"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="29"/>
       <c r="H14" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="29"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="48"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="25" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -1476,60 +1827,60 @@
       <c r="E16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="28"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="17"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="28"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="17"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="29"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="16"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="25" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -1538,58 +1889,58 @@
       <c r="E20" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="29"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="25" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -1598,60 +1949,60 @@
       <c r="E24" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="28"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="28"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="29"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="36" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -1660,10 +2011,10 @@
       <c r="E28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="33" t="s">
         <v>50</v>
       </c>
       <c r="H28" t="s">
@@ -1671,63 +2022,63 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="18"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="36"/>
       <c r="D29" s="3" t="s">
         <v>115</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="3" t="s">
         <v>117</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
       <c r="D31" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
       <c r="D32" s="2" t="s">
         <v>121</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="19" t="s">
+      <c r="A33" s="31"/>
+      <c r="B33" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="36" t="s">
         <v>122</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -1736,71 +2087,71 @@
       <c r="E33" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="33" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="18"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="36"/>
       <c r="D34" s="3" t="s">
         <v>129</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F34" s="18"/>
-      <c r="G34" s="19"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="33"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="31"/>
+      <c r="B38" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="25" t="s">
         <v>128</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -1809,71 +2160,71 @@
       <c r="E38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F38" s="27" t="s">
+      <c r="F38" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="28"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="28"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="3" t="s">
         <v>130</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="28"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="32"/>
       <c r="D41" s="3" t="s">
         <v>117</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="29"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="26"/>
       <c r="D42" s="3" t="s">
         <v>120</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="15" t="s">
+      <c r="A43" s="31"/>
+      <c r="B43" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="21" t="s">
         <v>83</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -1882,47 +2233,47 @@
       <c r="E43" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F43" s="27" t="s">
+      <c r="F43" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="G43" s="15" t="s">
+      <c r="G43" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F44" s="28"/>
-      <c r="G44" s="17"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
       <c r="D45" s="4" t="s">
         <v>137</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F45" s="29"/>
-      <c r="G45" s="16"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="22"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="36" t="s">
         <v>133</v>
       </c>
       <c r="D46" s="3" t="s">
@@ -1931,45 +2282,45 @@
       <c r="E46" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F46" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="G46" s="19" t="s">
+      <c r="G46" s="33" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="18"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="36"/>
       <c r="D47" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F47" s="18"/>
-      <c r="G47" s="19"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="33"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="18"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="36"/>
       <c r="D48" s="4" t="s">
         <v>140</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="19"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="33"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="15" t="s">
+      <c r="A49" s="31"/>
+      <c r="B49" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="25" t="s">
         <v>134</v>
       </c>
       <c r="D49" s="3" t="s">
@@ -1978,47 +2329,47 @@
       <c r="E49" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="27" t="s">
+      <c r="F49" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="28"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F50" s="28"/>
-      <c r="G50" s="17"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="29"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="26"/>
       <c r="D51" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="29"/>
-      <c r="G51" s="16"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="22"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="27" t="s">
+      <c r="C52" s="25" t="s">
         <v>142</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -2027,71 +2378,71 @@
       <c r="E52" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F52" s="27" t="s">
+      <c r="F52" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="G52" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="31"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="32"/>
       <c r="D53" s="3" t="s">
         <v>144</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F53" s="28"/>
-      <c r="G53" s="17"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="27"/>
     </row>
     <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="28"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="32"/>
       <c r="D54" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F54" s="28"/>
-      <c r="G54" s="17"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="27"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="28"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="32"/>
       <c r="D55" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F55" s="28"/>
-      <c r="G55" s="17"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="27"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="29"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="26"/>
       <c r="D56" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="29"/>
-      <c r="G56" s="16"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="22"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="11"/>
-      <c r="B57" s="15" t="s">
+      <c r="A57" s="31"/>
+      <c r="B57" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="27" t="s">
+      <c r="C57" s="25" t="s">
         <v>143</v>
       </c>
       <c r="D57" s="3" t="s">
@@ -2100,10 +2451,10 @@
       <c r="E57" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="27" t="s">
+      <c r="F57" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="G57" s="46" t="s">
+      <c r="G57" s="28" t="s">
         <v>50</v>
       </c>
       <c r="H57" t="s">
@@ -2111,65 +2462,65 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="28"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="32"/>
       <c r="D58" s="3" t="s">
         <v>144</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F58" s="28"/>
-      <c r="G58" s="47"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="29"/>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="28"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="32"/>
       <c r="D59" s="3" t="s">
         <v>148</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F59" s="28"/>
-      <c r="G59" s="47"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="29"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="28"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="32"/>
       <c r="D60" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F60" s="28"/>
-      <c r="G60" s="47"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="29"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="29"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="26"/>
       <c r="D61" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F61" s="29"/>
-      <c r="G61" s="48"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="30"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="27" t="s">
+      <c r="C62" s="25" t="s">
         <v>153</v>
       </c>
       <c r="D62" s="3" t="s">
@@ -2178,71 +2529,71 @@
       <c r="E62" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F62" s="27" t="s">
+      <c r="F62" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="G62" s="15" t="s">
+      <c r="G62" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="28"/>
+      <c r="A63" s="31"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="32"/>
       <c r="D63" s="3" t="s">
         <v>157</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F63" s="28"/>
-      <c r="G63" s="17"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="27"/>
     </row>
     <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="28"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="32"/>
       <c r="D64" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F64" s="28"/>
-      <c r="G64" s="17"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="27"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="28"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="32"/>
       <c r="D65" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="28"/>
-      <c r="G65" s="17"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="27"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="29"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="26"/>
       <c r="D66" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="29"/>
-      <c r="G66" s="16"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="22"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
-      <c r="B67" s="15" t="s">
+      <c r="A67" s="31"/>
+      <c r="B67" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C67" s="27" t="s">
+      <c r="C67" s="25" t="s">
         <v>154</v>
       </c>
       <c r="D67" s="3" t="s">
@@ -2251,10 +2602,10 @@
       <c r="E67" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F67" s="27" t="s">
+      <c r="F67" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="G67" s="46" t="s">
+      <c r="G67" s="28" t="s">
         <v>50</v>
       </c>
       <c r="H67" t="s">
@@ -2262,65 +2613,65 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="28"/>
+      <c r="A68" s="31"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="32"/>
       <c r="D68" s="3" t="s">
         <v>157</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F68" s="28"/>
-      <c r="G68" s="47"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="29"/>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="28"/>
+      <c r="A69" s="31"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="32"/>
       <c r="D69" s="3" t="s">
         <v>159</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F69" s="28"/>
-      <c r="G69" s="47"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="29"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="28"/>
+      <c r="A70" s="31"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="32"/>
       <c r="D70" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F70" s="28"/>
-      <c r="G70" s="47"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="29"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="29"/>
+      <c r="A71" s="24"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="26"/>
       <c r="D71" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F71" s="29"/>
-      <c r="G71" s="48"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="30"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C72" s="27" t="s">
+      <c r="C72" s="25" t="s">
         <v>161</v>
       </c>
       <c r="D72" s="3" t="s">
@@ -2329,34 +2680,34 @@
       <c r="E72" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F72" s="27" t="s">
+      <c r="F72" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="G72" s="15" t="s">
+      <c r="G72" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="29"/>
+      <c r="A73" s="24"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="26"/>
       <c r="D73" s="3" t="s">
         <v>165</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F73" s="29"/>
-      <c r="G73" s="16"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="22"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C74" s="27" t="s">
+      <c r="C74" s="25" t="s">
         <v>167</v>
       </c>
       <c r="D74" s="3" t="s">
@@ -2365,423 +2716,1926 @@
       <c r="E74" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F74" s="27" t="s">
+      <c r="F74" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="G74" s="15" t="s">
+      <c r="G74" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="29"/>
+      <c r="A75" s="24"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="26"/>
       <c r="D75" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="F75" s="29"/>
-      <c r="G75" s="16"/>
-    </row>
-    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="30" t="s">
+      <c r="F75" s="26"/>
+      <c r="G75" s="22"/>
+    </row>
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="G76" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F77" s="32"/>
+      <c r="G77" s="27"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="31"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F78" s="32"/>
+      <c r="G78" s="27"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="31"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F79" s="32"/>
+      <c r="G79" s="27"/>
+    </row>
+    <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="31"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="32"/>
+      <c r="G80" s="27"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="31"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="32"/>
+      <c r="G81" s="27"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="31"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="26"/>
+      <c r="G82" s="22"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
+      <c r="B83" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F83" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="G83" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F84" s="32"/>
+      <c r="G84" s="54"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F85" s="32"/>
+      <c r="G85" s="54"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="31"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F86" s="32"/>
+      <c r="G86" s="54"/>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="31"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="32"/>
+      <c r="G87" s="54"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="31"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="32"/>
+      <c r="G88" s="54"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="31"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="26"/>
+      <c r="G89" s="35"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="31"/>
+      <c r="B90" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F90" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="G90" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="31"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F91" s="32"/>
+      <c r="G91" s="27"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F92" s="32"/>
+      <c r="G92" s="27"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="31"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="26"/>
+      <c r="D93" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" s="26"/>
+      <c r="G93" s="22"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="31"/>
+      <c r="B94" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C94" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F94" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="G94" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="31"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F95" s="32"/>
+      <c r="G95" s="27"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="31"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F96" s="32"/>
+      <c r="G96" s="27"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="31"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F97" s="32"/>
+      <c r="G97" s="27"/>
+    </row>
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" s="32"/>
+      <c r="G98" s="27"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="31"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" s="32"/>
+      <c r="G99" s="27"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="31"/>
+      <c r="B100" s="22"/>
+      <c r="C100" s="26"/>
+      <c r="D100" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="26"/>
+      <c r="G100" s="22"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
+      <c r="B101" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="C101" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F101" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="G101" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H101" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="31"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F102" s="32"/>
+      <c r="G102" s="29"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="31"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F103" s="32"/>
+      <c r="G103" s="29"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="31"/>
+      <c r="B104" s="27"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F104" s="32"/>
+      <c r="G104" s="29"/>
+    </row>
+    <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="31"/>
+      <c r="B105" s="27"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="32"/>
+      <c r="G105" s="29"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F106" s="32"/>
+      <c r="G106" s="29"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
+      <c r="B107" s="22"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="26"/>
+      <c r="G107" s="30"/>
+    </row>
+    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C108" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F108" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="G108" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="31"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="32"/>
+      <c r="D109" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F109" s="32"/>
+      <c r="G109" s="27"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="31"/>
+      <c r="B110" s="27"/>
+      <c r="C110" s="32"/>
+      <c r="D110" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F110" s="32"/>
+      <c r="G110" s="27"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="31"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="32"/>
+      <c r="D111" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F111" s="32"/>
+      <c r="G111" s="27"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="31"/>
+      <c r="B112" s="27"/>
+      <c r="C112" s="32"/>
+      <c r="D112" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F112" s="32"/>
+      <c r="G112" s="27"/>
+    </row>
+    <row r="113" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="31"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="32"/>
+      <c r="D113" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F113" s="32"/>
+      <c r="G113" s="27"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="31"/>
+      <c r="B114" s="22"/>
+      <c r="C114" s="26"/>
+      <c r="D114" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F114" s="26"/>
+      <c r="G114" s="22"/>
+    </row>
+    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="31"/>
+      <c r="B115" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C115" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F115" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="G115" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="31"/>
+      <c r="B116" s="27"/>
+      <c r="C116" s="32"/>
+      <c r="D116" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F116" s="32"/>
+      <c r="G116" s="27"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="31"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="32"/>
+      <c r="D117" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F117" s="32"/>
+      <c r="G117" s="27"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
+      <c r="B118" s="27"/>
+      <c r="C118" s="32"/>
+      <c r="D118" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F118" s="32"/>
+      <c r="G118" s="27"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
+      <c r="B119" s="27"/>
+      <c r="C119" s="32"/>
+      <c r="D119" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F119" s="32"/>
+      <c r="G119" s="27"/>
+    </row>
+    <row r="120" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="31"/>
+      <c r="B120" s="27"/>
+      <c r="C120" s="32"/>
+      <c r="D120" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="32"/>
+      <c r="G120" s="27"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="31"/>
+      <c r="B121" s="22"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F121" s="26"/>
+      <c r="G121" s="22"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="31"/>
+      <c r="B122" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C122" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F122" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="G122" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
+      <c r="B123" s="27"/>
+      <c r="C123" s="32"/>
+      <c r="D123" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F123" s="32"/>
+      <c r="G123" s="27"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
+      <c r="B124" s="27"/>
+      <c r="C124" s="32"/>
+      <c r="D124" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F124" s="32"/>
+      <c r="G124" s="27"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
+      <c r="B125" s="27"/>
+      <c r="C125" s="32"/>
+      <c r="D125" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F125" s="32"/>
+      <c r="G125" s="27"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
+      <c r="B126" s="27"/>
+      <c r="C126" s="32"/>
+      <c r="D126" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F126" s="32"/>
+      <c r="G126" s="27"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="31"/>
+      <c r="B127" s="27"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F127" s="32"/>
+      <c r="G127" s="27"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="31"/>
+      <c r="B128" s="27"/>
+      <c r="C128" s="32"/>
+      <c r="D128" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" s="32"/>
+      <c r="G128" s="27"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="31"/>
+      <c r="B129" s="22"/>
+      <c r="C129" s="26"/>
+      <c r="D129" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F129" s="26"/>
+      <c r="G129" s="22"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="31"/>
+      <c r="B130" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="C130" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F130" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="G130" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H130" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="31"/>
+      <c r="B131" s="27"/>
+      <c r="C131" s="32"/>
+      <c r="D131" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F131" s="32"/>
+      <c r="G131" s="29"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="31"/>
+      <c r="B132" s="27"/>
+      <c r="C132" s="32"/>
+      <c r="D132" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F132" s="32"/>
+      <c r="G132" s="29"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="31"/>
+      <c r="B133" s="27"/>
+      <c r="C133" s="32"/>
+      <c r="D133" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F133" s="32"/>
+      <c r="G133" s="29"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="31"/>
+      <c r="B134" s="27"/>
+      <c r="C134" s="32"/>
+      <c r="D134" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E134" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F134" s="32"/>
+      <c r="G134" s="29"/>
+    </row>
+    <row r="135" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="31"/>
+      <c r="B135" s="27"/>
+      <c r="C135" s="32"/>
+      <c r="D135" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" s="32"/>
+      <c r="G135" s="29"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="31"/>
+      <c r="B136" s="27"/>
+      <c r="C136" s="32"/>
+      <c r="D136" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F136" s="32"/>
+      <c r="G136" s="29"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="31"/>
+      <c r="B137" s="22"/>
+      <c r="C137" s="26"/>
+      <c r="D137" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F137" s="26"/>
+      <c r="G137" s="30"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="B138" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C138" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F138" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="G138" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="31"/>
+      <c r="B139" s="27"/>
+      <c r="C139" s="32"/>
+      <c r="D139" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F139" s="32"/>
+      <c r="G139" s="54"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="31"/>
+      <c r="B140" s="27"/>
+      <c r="C140" s="32"/>
+      <c r="D140" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F140" s="32"/>
+      <c r="G140" s="54"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="31"/>
+      <c r="B141" s="27"/>
+      <c r="C141" s="32"/>
+      <c r="D141" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F141" s="32"/>
+      <c r="G141" s="54"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="31"/>
+      <c r="B142" s="27"/>
+      <c r="C142" s="32"/>
+      <c r="D142" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F142" s="32"/>
+      <c r="G142" s="54"/>
+    </row>
+    <row r="143" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A143" s="31"/>
+      <c r="B143" s="27"/>
+      <c r="C143" s="32"/>
+      <c r="D143" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="32"/>
+      <c r="G143" s="54"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="31"/>
+      <c r="B144" s="22"/>
+      <c r="C144" s="26"/>
+      <c r="D144" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E144" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F144" s="26"/>
+      <c r="G144" s="35"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="31"/>
+      <c r="B145" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C145" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F145" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="G145" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="31"/>
+      <c r="B146" s="27"/>
+      <c r="C146" s="32"/>
+      <c r="D146" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E146" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F146" s="32"/>
+      <c r="G146" s="54"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="31"/>
+      <c r="B147" s="27"/>
+      <c r="C147" s="32"/>
+      <c r="D147" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F147" s="32"/>
+      <c r="G147" s="54"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="31"/>
+      <c r="B148" s="27"/>
+      <c r="C148" s="32"/>
+      <c r="D148" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E148" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F148" s="32"/>
+      <c r="G148" s="54"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="31"/>
+      <c r="B149" s="27"/>
+      <c r="C149" s="32"/>
+      <c r="D149" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F149" s="32"/>
+      <c r="G149" s="54"/>
+    </row>
+    <row r="150" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="31"/>
+      <c r="B150" s="27"/>
+      <c r="C150" s="32"/>
+      <c r="D150" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F150" s="32"/>
+      <c r="G150" s="54"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="31"/>
+      <c r="B151" s="22"/>
+      <c r="C151" s="26"/>
+      <c r="D151" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F151" s="26"/>
+      <c r="G151" s="35"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="31"/>
+      <c r="B152" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C152" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F152" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="G152" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="31"/>
+      <c r="B153" s="27"/>
+      <c r="C153" s="32"/>
+      <c r="D153" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F153" s="32"/>
+      <c r="G153" s="54"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="31"/>
+      <c r="B154" s="27"/>
+      <c r="C154" s="32"/>
+      <c r="D154" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E154" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F154" s="32"/>
+      <c r="G154" s="54"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="31"/>
+      <c r="B155" s="27"/>
+      <c r="C155" s="32"/>
+      <c r="D155" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F155" s="32"/>
+      <c r="G155" s="54"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="31"/>
+      <c r="B156" s="27"/>
+      <c r="C156" s="32"/>
+      <c r="D156" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E156" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F156" s="32"/>
+      <c r="G156" s="54"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="31"/>
+      <c r="B157" s="27"/>
+      <c r="C157" s="32"/>
+      <c r="D157" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F157" s="32"/>
+      <c r="G157" s="54"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="24"/>
+      <c r="B158" s="22"/>
+      <c r="C158" s="26"/>
+      <c r="D158" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F158" s="26"/>
+      <c r="G158" s="35"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B159" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="C159" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F159" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="G159" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="31"/>
+      <c r="B160" s="27"/>
+      <c r="C160" s="32"/>
+      <c r="D160" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F160" s="32"/>
+      <c r="G160" s="54"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="31"/>
+      <c r="B161" s="27"/>
+      <c r="C161" s="32"/>
+      <c r="D161" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F161" s="32"/>
+      <c r="G161" s="54"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="31"/>
+      <c r="B162" s="22"/>
+      <c r="C162" s="26"/>
+      <c r="D162" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F162" s="26"/>
+      <c r="G162" s="35"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="31"/>
+      <c r="B163" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="C163" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F163" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="G163" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="31"/>
+      <c r="B164" s="27"/>
+      <c r="C164" s="32"/>
+      <c r="D164" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E164" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F164" s="32"/>
+      <c r="G164" s="54"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="31"/>
+      <c r="B165" s="27"/>
+      <c r="C165" s="32"/>
+      <c r="D165" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F165" s="32"/>
+      <c r="G165" s="54"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="24"/>
+      <c r="B166" s="22"/>
+      <c r="C166" s="26"/>
+      <c r="D166" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F166" s="26"/>
+      <c r="G166" s="35"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="B167" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C167" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E167" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F167" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="G167" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="31"/>
+      <c r="B168" s="27"/>
+      <c r="C168" s="32"/>
+      <c r="D168" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E168" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F168" s="32"/>
+      <c r="G168" s="54"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="31"/>
+      <c r="B169" s="22"/>
+      <c r="C169" s="26"/>
+      <c r="D169" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E169" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F169" s="26"/>
+      <c r="G169" s="35"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="31"/>
+      <c r="B170" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="C170" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E170" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F170" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="G170" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="31"/>
+      <c r="B171" s="27"/>
+      <c r="C171" s="32"/>
+      <c r="D171" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F171" s="32"/>
+      <c r="G171" s="54"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="31"/>
+      <c r="B172" s="27"/>
+      <c r="C172" s="32"/>
+      <c r="D172" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E172" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F172" s="32"/>
+      <c r="G172" s="54"/>
+    </row>
+    <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="24"/>
+      <c r="B173" s="22"/>
+      <c r="C173" s="26"/>
+      <c r="D173" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F173" s="26"/>
+      <c r="G173" s="35"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="10"/>
+      <c r="B174" s="12"/>
+      <c r="C174" s="16"/>
+      <c r="D174" s="3"/>
+      <c r="E174" s="4"/>
+      <c r="F174" s="16"/>
+      <c r="G174" s="11"/>
+    </row>
+    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B76" s="31" t="s">
+      <c r="B175" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C76" s="31" t="s">
+      <c r="C175" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="D76" s="32" t="s">
+      <c r="D175" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E76" s="33" t="s">
+      <c r="E175" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F76" s="34" t="s">
+      <c r="F175" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="G76" s="31" t="s">
+      <c r="G175" s="45" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="35"/>
-      <c r="B77" s="31"/>
-      <c r="C77" s="31"/>
-      <c r="D77" s="33" t="s">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="52"/>
+      <c r="B176" s="45"/>
+      <c r="C176" s="45"/>
+      <c r="D176" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E77" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="35"/>
-      <c r="B78" s="31"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="33" t="s">
+      <c r="E176" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F176" s="45"/>
+      <c r="G176" s="45"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="52"/>
+      <c r="B177" s="45"/>
+      <c r="C177" s="45"/>
+      <c r="D177" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E78" s="33" t="s">
+      <c r="E177" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="35"/>
-      <c r="B79" s="31"/>
-      <c r="C79" s="31"/>
-      <c r="D79" s="33" t="s">
+      <c r="F177" s="45"/>
+      <c r="G177" s="45"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="52"/>
+      <c r="B178" s="45"/>
+      <c r="C178" s="45"/>
+      <c r="D178" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E79" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="33" t="s">
+      <c r="E178" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F178" s="45"/>
+      <c r="G178" s="45"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="52"/>
+      <c r="B179" s="45"/>
+      <c r="C179" s="45"/>
+      <c r="D179" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E80" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="35"/>
-      <c r="B81" s="31" t="s">
+      <c r="E179" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F179" s="45"/>
+      <c r="G179" s="45"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="52"/>
+      <c r="B180" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C81" s="31" t="s">
+      <c r="C180" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="D81" s="33" t="s">
+      <c r="D180" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E81" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="34" t="s">
+      <c r="E180" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F180" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="G81" s="36" t="s">
+      <c r="G180" s="41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="35"/>
-      <c r="B82" s="31"/>
-      <c r="C82" s="31"/>
-      <c r="D82" s="33" t="s">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="52"/>
+      <c r="B181" s="45"/>
+      <c r="C181" s="45"/>
+      <c r="D181" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E82" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="34"/>
-      <c r="G82" s="37"/>
-    </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="35"/>
-      <c r="B83" s="31" t="s">
+      <c r="E181" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" s="44"/>
+      <c r="G181" s="42"/>
+    </row>
+    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" s="52"/>
+      <c r="B182" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C83" s="31" t="s">
+      <c r="C182" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="D83" s="32" t="s">
+      <c r="D182" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E83" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="34" t="s">
+      <c r="E182" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F182" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="G83" s="31" t="s">
+      <c r="G182" s="45" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="38"/>
-      <c r="B84" s="31"/>
-      <c r="C84" s="31"/>
-      <c r="D84" s="33" t="s">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="53"/>
+      <c r="B183" s="45"/>
+      <c r="C183" s="45"/>
+      <c r="D183" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E84" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="34"/>
-      <c r="G84" s="31"/>
-    </row>
-    <row r="85" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="39" t="s">
+      <c r="E183" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F183" s="44"/>
+      <c r="G183" s="45"/>
+    </row>
+    <row r="184" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B85" s="31" t="s">
+      <c r="B184" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C85" s="31" t="s">
+      <c r="C184" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D85" s="33" t="s">
+      <c r="D184" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E85" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="34" t="s">
+      <c r="E184" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F184" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="G85" s="36" t="s">
+      <c r="G184" s="41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="40"/>
-      <c r="B86" s="31"/>
-      <c r="C86" s="31"/>
-      <c r="D86" s="33" t="s">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="49"/>
+      <c r="B185" s="45"/>
+      <c r="C185" s="45"/>
+      <c r="D185" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E86" s="33" t="s">
+      <c r="E185" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F86" s="31"/>
-      <c r="G86" s="41"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="40"/>
-      <c r="B87" s="31"/>
-      <c r="C87" s="31"/>
-      <c r="D87" s="33" t="s">
+      <c r="F185" s="45"/>
+      <c r="G185" s="43"/>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="49"/>
+      <c r="B186" s="45"/>
+      <c r="C186" s="45"/>
+      <c r="D186" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E87" s="33" t="s">
+      <c r="E186" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F87" s="31"/>
-      <c r="G87" s="37"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="40"/>
-      <c r="B88" s="31" t="s">
+      <c r="F186" s="45"/>
+      <c r="G186" s="42"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="49"/>
+      <c r="B187" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="C88" s="31" t="s">
+      <c r="C187" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="D88" s="33" t="s">
+      <c r="D187" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E88" s="33" t="s">
+      <c r="E187" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F88" s="34" t="s">
+      <c r="F187" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="G88" s="36" t="s">
+      <c r="G187" s="41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="40"/>
-      <c r="B89" s="31"/>
-      <c r="C89" s="31"/>
-      <c r="D89" s="33" t="s">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" s="49"/>
+      <c r="B188" s="45"/>
+      <c r="C188" s="45"/>
+      <c r="D188" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E89" s="33" t="s">
+      <c r="E188" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F89" s="31"/>
-      <c r="G89" s="37"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="42"/>
-      <c r="B90" s="43" t="s">
+      <c r="F188" s="45"/>
+      <c r="G188" s="42"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="50"/>
+      <c r="B189" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C90" s="43" t="s">
+      <c r="C189" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D90" s="33" t="s">
+      <c r="D189" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E90" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="43" t="s">
+      <c r="E189" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F189" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G90" s="43" t="s">
+      <c r="G189" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="44" t="s">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="B91" s="43" t="s">
+      <c r="B190" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C91" s="45" t="s">
+      <c r="C190" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D91" s="33" t="s">
+      <c r="D190" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E91" s="33" t="s">
+      <c r="E190" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F91" s="45" t="s">
+      <c r="F190" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G91" s="45" t="s">
+      <c r="G190" s="20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
-      <c r="B92" s="43" t="s">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" s="47"/>
+      <c r="B191" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="45" t="s">
+      <c r="C191" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D92" s="33" t="s">
+      <c r="D191" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E92" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="45" t="s">
+      <c r="E191" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F191" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="G92" s="45" t="s">
+      <c r="G191" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B192" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C93" s="27" t="s">
+      <c r="C192" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="D93" s="6" t="s">
+      <c r="D192" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E93" s="6" t="s">
+      <c r="E192" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F93" s="15" t="s">
+      <c r="F192" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G93" s="15" t="s">
+      <c r="G192" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="11"/>
-      <c r="B94" s="16"/>
-      <c r="C94" s="16"/>
-      <c r="D94" s="6" t="s">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" s="31"/>
+      <c r="B193" s="22"/>
+      <c r="C193" s="22"/>
+      <c r="D193" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E94" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F94" s="16"/>
-      <c r="G94" s="16"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="11"/>
-      <c r="B95" s="13" t="s">
+      <c r="E193" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F193" s="22"/>
+      <c r="G193" s="22"/>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="31"/>
+      <c r="B194" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="C95" s="49" t="s">
+      <c r="C194" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="D95" s="6" t="s">
+      <c r="D194" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="6" t="s">
+      <c r="E194" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="F95" s="15" t="s">
+      <c r="F194" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G95" s="13" t="s">
+      <c r="G194" s="46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="6" t="s">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" s="24"/>
+      <c r="B195" s="35"/>
+      <c r="C195" s="35"/>
+      <c r="D195" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E96" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F96" s="16"/>
-      <c r="G96" s="14"/>
+      <c r="E195" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F195" s="22"/>
+      <c r="G195" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="114">
-    <mergeCell ref="G93:G94"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="G72:G73"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="G57:G61"/>
-    <mergeCell ref="A62:A71"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="C62:C66"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="C67:C71"/>
-    <mergeCell ref="F62:F66"/>
-    <mergeCell ref="F67:F71"/>
-    <mergeCell ref="G62:G66"/>
-    <mergeCell ref="G67:G71"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="F38:F42"/>
-    <mergeCell ref="G38:G42"/>
+  <mergeCells count="183">
+    <mergeCell ref="A167:A173"/>
+    <mergeCell ref="F167:F169"/>
+    <mergeCell ref="G167:G169"/>
+    <mergeCell ref="B167:B169"/>
+    <mergeCell ref="C167:C169"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="F170:F173"/>
+    <mergeCell ref="G170:G173"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="A138:A158"/>
+    <mergeCell ref="F159:F162"/>
+    <mergeCell ref="G159:G162"/>
+    <mergeCell ref="C159:C162"/>
+    <mergeCell ref="B159:B162"/>
+    <mergeCell ref="C163:C166"/>
+    <mergeCell ref="B163:B166"/>
+    <mergeCell ref="F163:F166"/>
+    <mergeCell ref="G163:G166"/>
+    <mergeCell ref="A159:A166"/>
+    <mergeCell ref="C138:C144"/>
+    <mergeCell ref="B138:B144"/>
+    <mergeCell ref="F138:F144"/>
+    <mergeCell ref="F145:F151"/>
+    <mergeCell ref="C145:C151"/>
+    <mergeCell ref="B145:B151"/>
+    <mergeCell ref="G138:G144"/>
+    <mergeCell ref="G145:G151"/>
+    <mergeCell ref="C152:C158"/>
+    <mergeCell ref="F152:F158"/>
+    <mergeCell ref="G152:G158"/>
+    <mergeCell ref="B152:B158"/>
+    <mergeCell ref="A108:A137"/>
+    <mergeCell ref="C108:C114"/>
+    <mergeCell ref="C115:C121"/>
+    <mergeCell ref="B108:B114"/>
+    <mergeCell ref="B115:B121"/>
+    <mergeCell ref="F108:F114"/>
+    <mergeCell ref="F115:F121"/>
+    <mergeCell ref="G108:G114"/>
+    <mergeCell ref="G115:G121"/>
+    <mergeCell ref="F122:F129"/>
+    <mergeCell ref="G122:G129"/>
+    <mergeCell ref="C122:C129"/>
+    <mergeCell ref="B122:B129"/>
+    <mergeCell ref="C130:C137"/>
+    <mergeCell ref="B130:B137"/>
+    <mergeCell ref="F130:F137"/>
+    <mergeCell ref="G130:G137"/>
+    <mergeCell ref="F94:F100"/>
+    <mergeCell ref="G94:G100"/>
+    <mergeCell ref="C94:C100"/>
+    <mergeCell ref="B94:B100"/>
+    <mergeCell ref="F101:F107"/>
+    <mergeCell ref="G101:G107"/>
+    <mergeCell ref="C101:C107"/>
+    <mergeCell ref="B101:B107"/>
+    <mergeCell ref="A76:A107"/>
+    <mergeCell ref="B175:B179"/>
+    <mergeCell ref="C175:C179"/>
+    <mergeCell ref="C180:C181"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="B76:B82"/>
+    <mergeCell ref="C76:C82"/>
+    <mergeCell ref="F76:F82"/>
+    <mergeCell ref="G76:G82"/>
+    <mergeCell ref="C83:C89"/>
+    <mergeCell ref="B83:B89"/>
+    <mergeCell ref="F83:F89"/>
+    <mergeCell ref="F90:F93"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="G83:G89"/>
+    <mergeCell ref="G90:G93"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A28:A45"/>
+    <mergeCell ref="G187:G188"/>
+    <mergeCell ref="G184:G186"/>
+    <mergeCell ref="F182:F183"/>
+    <mergeCell ref="G182:G183"/>
+    <mergeCell ref="C182:C183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="B184:B186"/>
+    <mergeCell ref="F187:F188"/>
+    <mergeCell ref="C187:C188"/>
+    <mergeCell ref="B187:B188"/>
+    <mergeCell ref="F184:F186"/>
+    <mergeCell ref="C184:C186"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="G175:G179"/>
+    <mergeCell ref="G180:G181"/>
+    <mergeCell ref="A184:A189"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="A52:A61"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="F52:F56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="C46:C48"/>
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B24:B27"/>
@@ -2800,68 +4654,61 @@
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="C16:C19"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="F38:F42"/>
+    <mergeCell ref="G38:G42"/>
     <mergeCell ref="F28:F32"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A93:A96"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="A52:A61"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="F52:F56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="C57:C61"/>
     <mergeCell ref="F33:F37"/>
     <mergeCell ref="G33:G37"/>
     <mergeCell ref="G28:G32"/>
-    <mergeCell ref="B46:B48"/>
     <mergeCell ref="B33:B37"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="C28:C32"/>
     <mergeCell ref="C33:C37"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A28:A45"/>
-    <mergeCell ref="G88:G89"/>
-    <mergeCell ref="G85:G87"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="G83:G84"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B85:B87"/>
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="F85:F87"/>
-    <mergeCell ref="C85:C87"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="G76:G80"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="F95:F96"/>
-    <mergeCell ref="G95:G96"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A85:A90"/>
-    <mergeCell ref="A76:A84"/>
-    <mergeCell ref="F76:F80"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="A62:A71"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="C62:C66"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="C67:C71"/>
+    <mergeCell ref="F62:F66"/>
+    <mergeCell ref="F67:F71"/>
+    <mergeCell ref="G62:G66"/>
+    <mergeCell ref="G67:G71"/>
+    <mergeCell ref="G192:G193"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="G72:G73"/>
+    <mergeCell ref="F192:F193"/>
+    <mergeCell ref="A192:A195"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="B194:B195"/>
+    <mergeCell ref="F194:F195"/>
+    <mergeCell ref="G194:G195"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="A175:A183"/>
+    <mergeCell ref="F175:F179"/>
+    <mergeCell ref="F180:F181"/>
+    <mergeCell ref="B180:B181"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>